<commit_message>
add name column to template
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Test Data</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -470,7 +473,7 @@
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -479,6 +482,9 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>